<commit_message>
Update: read keys from excel
</commit_message>
<xml_diff>
--- a/Mapping/unimelb_parkville_url.xlsx
+++ b/Mapping/unimelb_parkville_url.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud-my.sharepoint.com/personal/boat_amorntiyanggoon_unimelb_edu_au/Documents/Casual Tasks/URL_extraction/mapping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HYC-MacBookPro/Documents/Digital Estate/hyperlink-pasting/Mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_530D03F05FA348AC551371AA2DED170B78790007" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03FAC901-F50C-4905-BC8A-8D78530E2D80}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B893740D-0148-CF4D-B6F7-7BAA4BBB50CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1450,16 +1450,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>57</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>62</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>68</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>69</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>71</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>72</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>73</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>74</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>75</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>76</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>77</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>78</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>79</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>80</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>81</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>82</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>83</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>84</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>85</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>86</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>87</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>88</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>89</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>90</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>91</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>92</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>93</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>94</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>95</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>96</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>97</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>98</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>99</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>100</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>101</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>102</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>103</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>104</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>105</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>105</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>106</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>107</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>108</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>109</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>110</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>111</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>112</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>113</v>
       </c>

</xml_diff>